<commit_message>
Genomgång, kontroll och refaktorering av testfall.
</commit_message>
<xml_diff>
--- a/documents/Item_Beslutstabell.xlsx
+++ b/documents/Item_Beslutstabell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jon/Programmering/GitHub/INTE-spelet/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A334DBC1-3D01-EC41-BC78-B093628514E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000245D9-015F-F341-A030-6BA76B3E9148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{E0BCFC50-83D9-EA44-9C0D-3790F3676A66}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{E0BCFC50-83D9-EA44-9C0D-3790F3676A66}"/>
   </bookViews>
   <sheets>
     <sheet name="Item x Character" sheetId="2" r:id="rId1"/>
@@ -828,7 +828,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection sqref="A1:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1598,6 +1598,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -1856,6 +1857,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2064,5 +2066,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>